<commit_message>
since byron added new model, change table logic so we get it
</commit_message>
<xml_diff>
--- a/How-To/iCARE Template (Client Profile) MODIFIED.xlsx
+++ b/How-To/iCARE Template (Client Profile) MODIFIED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dharmik\Desktop\Team20\How-To\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2D73F1-FFAF-436C-8F10-F9B50B2D1BBF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4533488A-DA35-44AB-B3EB-2CB085706019}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3525" yWindow="465" windowWidth="24600" windowHeight="16545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,7 +186,7 @@
     <t>M6G3A4</t>
   </si>
   <si>
-    <t>8819382</t>
+    <t>881938200</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:Q2503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48342,8 +48342,11 @@
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:Q3" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B31 J4:J35 P4:P42 N4:N35 K4:K36 F4:F43 Q4:Q34" xr:uid="{00000000-0002-0000-0200-000008000000}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{30524E1E-4AB6-4BC3-8F35-44BE53679CBC}"/>
@@ -48351,49 +48354,13 @@
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'xlFile://Root/CurrentDir/[Client+Profile_Bulk+Upload+Template_2018-07-16_VER_794 (1).xlsx]LOV'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>Q35:Q2503 B32:B2503 F44:F2503 J36:J2503 K37:K2503 N36:N2503 P43:P2503</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000008000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B31</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000009000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F43 Q4:Q34</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-00000A000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>K4:K36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-00000B000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>N4:N35</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-00000C000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>P4:P42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-00000D000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J4:J35</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>